<commit_message>
Committed as on 17 Feb 2019
</commit_message>
<xml_diff>
--- a/src/Payless/TestData/Payless_GUITestData_CreateReservation.xlsx
+++ b/src/Payless/TestData/Payless_GUITestData_CreateReservation.xlsx
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2915" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="535">
   <si>
     <t>REGION</t>
   </si>
@@ -1855,6 +1855,54 @@
   </si>
   <si>
     <t>Reservation created successfully. Reservation Number: 05623629US4</t>
+  </si>
+  <si>
+    <t>Reservation created successfully. Reservation Number: 05623638US6</t>
+  </si>
+  <si>
+    <t>05623638US6</t>
+  </si>
+  <si>
+    <t>Reservation created successfully. Reservation Number: 05623641US2</t>
+  </si>
+  <si>
+    <t>05623641US2</t>
+  </si>
+  <si>
+    <t>$999.96</t>
+  </si>
+  <si>
+    <t>$1,224.81</t>
+  </si>
+  <si>
+    <t>05623644US5</t>
+  </si>
+  <si>
+    <t>$696.00</t>
+  </si>
+  <si>
+    <t>$139.92</t>
+  </si>
+  <si>
+    <t>$941.41</t>
+  </si>
+  <si>
+    <t>05623647US1</t>
+  </si>
+  <si>
+    <t>5K</t>
+  </si>
+  <si>
+    <t>12/10/18</t>
+  </si>
+  <si>
+    <t>5 Days 0 Hours</t>
+  </si>
+  <si>
+    <t>$144.16</t>
+  </si>
+  <si>
+    <t>$210.00</t>
   </si>
 </sst>
 </file>
@@ -8089,7 +8137,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>88</v>
+        <v>434</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>89</v>
@@ -8187,23 +8235,51 @@
       </c>
       <c r="AJ29" s="38"/>
       <c r="AK29" s="38"/>
-      <c r="AL29" s="8"/>
-      <c r="AM29" s="8"/>
-      <c r="AN29" s="8"/>
-      <c r="AO29" s="11"/>
-      <c r="AP29" s="8"/>
-      <c r="AQ29" s="8"/>
-      <c r="AR29" s="11"/>
-      <c r="AS29" s="8"/>
-      <c r="AT29" s="10"/>
-      <c r="AU29" s="10"/>
-      <c r="AV29" s="10"/>
-      <c r="AW29" s="10"/>
-      <c r="AX29" s="10"/>
+      <c r="AL29" s="8" t="s">
+        <v>520</v>
+      </c>
+      <c r="AM29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO29" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ29" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="AR29" s="11" t="s">
+        <v>504</v>
+      </c>
+      <c r="AS29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT29" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="AU29" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AV29" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AW29" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="AX29" s="10" t="s">
+        <v>512</v>
+      </c>
       <c r="AY29" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="AZ29" s="10"/>
+        <v>519</v>
+      </c>
+      <c r="AZ29" s="10" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A30" s="36" t="s">
@@ -8213,7 +8289,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>88</v>
+        <v>434</v>
       </c>
       <c r="D30" s="37" t="s">
         <v>89</v>
@@ -8311,21 +8387,51 @@
       </c>
       <c r="AJ30" s="38"/>
       <c r="AK30" s="38"/>
-      <c r="AL30" s="8"/>
-      <c r="AM30" s="8"/>
-      <c r="AN30" s="8"/>
-      <c r="AO30" s="8"/>
-      <c r="AP30" s="11"/>
-      <c r="AQ30" s="8"/>
-      <c r="AR30" s="8"/>
-      <c r="AS30" s="11"/>
-      <c r="AT30" s="8"/>
-      <c r="AU30" s="10"/>
-      <c r="AV30" s="10"/>
-      <c r="AW30" s="10"/>
-      <c r="AX30" s="10"/>
-      <c r="AY30" s="10"/>
-      <c r="AZ30" s="10"/>
+      <c r="AL30" s="8" t="s">
+        <v>522</v>
+      </c>
+      <c r="AM30" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN30" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO30" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AP30" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ30" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="AR30" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="AS30" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT30" s="8" t="s">
+        <v>523</v>
+      </c>
+      <c r="AU30" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AV30" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AW30" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="AX30" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="AY30" s="10" t="s">
+        <v>521</v>
+      </c>
+      <c r="AZ30" s="10" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="31" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A31" s="36" t="s">
@@ -8335,7 +8441,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>88</v>
+        <v>434</v>
       </c>
       <c r="D31" s="37" t="s">
         <v>89</v>
@@ -8433,21 +8539,51 @@
         <v>280</v>
       </c>
       <c r="AK31" s="38"/>
-      <c r="AL31" s="8"/>
-      <c r="AM31" s="8"/>
-      <c r="AN31" s="8"/>
-      <c r="AO31" s="8"/>
-      <c r="AP31" s="8"/>
-      <c r="AQ31" s="8"/>
-      <c r="AR31" s="8"/>
-      <c r="AS31" s="8"/>
-      <c r="AT31" s="10"/>
-      <c r="AU31" s="10"/>
-      <c r="AV31" s="10"/>
-      <c r="AW31" s="10"/>
-      <c r="AX31" s="10"/>
-      <c r="AY31" s="10"/>
-      <c r="AZ31" s="10"/>
+      <c r="AL31" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="AM31" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ31" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="AR31" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="AS31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT31" s="10" t="s">
+        <v>526</v>
+      </c>
+      <c r="AU31" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AV31" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="AW31" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="AX31" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="AY31" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="AZ31" s="10" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
@@ -8457,7 +8593,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>88</v>
+        <v>434</v>
       </c>
       <c r="D32" s="37" t="s">
         <v>89</v>
@@ -8555,21 +8691,51 @@
       </c>
       <c r="AJ32" s="4"/>
       <c r="AK32" s="4"/>
-      <c r="AL32" s="8"/>
-      <c r="AM32" s="8"/>
-      <c r="AN32" s="8"/>
-      <c r="AO32" s="11"/>
-      <c r="AP32" s="8"/>
-      <c r="AQ32" s="8"/>
-      <c r="AR32" s="11"/>
-      <c r="AS32" s="8"/>
-      <c r="AT32" s="10"/>
-      <c r="AU32" s="10"/>
-      <c r="AV32" s="10"/>
-      <c r="AW32" s="10"/>
-      <c r="AX32" s="10"/>
-      <c r="AY32" s="10"/>
-      <c r="AZ32" s="10"/>
+      <c r="AL32" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="AM32" s="8" t="s">
+        <v>530</v>
+      </c>
+      <c r="AN32" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO32" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AP32" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ32" s="8" t="s">
+        <v>424</v>
+      </c>
+      <c r="AR32" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="AS32" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="AT32" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="AU32" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AV32" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="AW32" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="AX32" s="10" t="s">
+        <v>534</v>
+      </c>
+      <c r="AY32" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="AZ32" s="10" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
@@ -8690,7 +8856,9 @@
       <c r="AV33" s="10"/>
       <c r="AW33" s="10"/>
       <c r="AX33" s="10"/>
-      <c r="AY33" s="10"/>
+      <c r="AY33" s="10" t="s">
+        <v>426</v>
+      </c>
       <c r="AZ33" s="10"/>
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">

</xml_diff>